<commit_message>
-pdf documents have been updated
</commit_message>
<xml_diff>
--- a/SuperDeniz/Images/Offers/ilk_insaat/superdeniz_teklif_formu.xlsx
+++ b/SuperDeniz/Images/Offers/ilk_insaat/superdeniz_teklif_formu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Osman\superdenizaydinlatma\SuperDeniz\Images\Offers\ilk_insaat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Osman\superdeniz\SuperDeniz\Images\Offers\ilk_insaat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E23363F7-43CF-4CB9-B2A1-3E0C8CFDC90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C85B9A-22D8-42E9-9A48-86F29800C808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A150985F-6D78-43E6-9132-8487C9950337}"/>
+    <workbookView xWindow="28680" yWindow="-180" windowWidth="29040" windowHeight="15840" xr2:uid="{A150985F-6D78-43E6-9132-8487C9950337}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="57">
   <si>
     <t>Adres</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>%50 peşin, %50 ürün teslim öncesi ödeme.</t>
+  </si>
+  <si>
+    <t>Proforma Fatura</t>
+  </si>
+  <si>
+    <t>Gebze Depo Adresi: Barış Mah. Anibal Cad. No:15 Gebze/KOCAELİ</t>
   </si>
 </sst>
 </file>
@@ -388,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -444,61 +450,64 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -511,13 +520,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -837,7 +840,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:J16"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -858,28 +861,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
       <c r="H1" s="7"/>
       <c r="K1" s="17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="7"/>
       <c r="I2" s="1" t="s">
         <v>0</v>
@@ -892,26 +895,26 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="7"/>
       <c r="K3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="7"/>
       <c r="I4" s="1" t="s">
         <v>4</v>
@@ -924,13 +927,13 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="7"/>
       <c r="I5" s="1" t="s">
         <v>6</v>
@@ -943,13 +946,13 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="7"/>
       <c r="I6" s="1" t="s">
         <v>8</v>
@@ -962,15 +965,15 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="3"/>
       <c r="I7" s="1" t="s">
         <v>10</v>
@@ -990,26 +993,26 @@
       <c r="J9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K9" s="40">
-        <v>44371</v>
-      </c>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="41"/>
+      <c r="K9" s="31">
+        <v>44390</v>
+      </c>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1024,7 +1027,7 @@
       <c r="I11" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="37" t="s">
+      <c r="J11" s="27" t="s">
         <v>1</v>
       </c>
       <c r="K11" s="26" t="s">
@@ -1045,12 +1048,12 @@
       <c r="G12" s="13"/>
       <c r="H12" s="6"/>
       <c r="I12" s="26"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
@@ -1063,119 +1066,119 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
+      <c r="A14" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
     </row>
     <row r="15" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
     </row>
     <row r="16" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
       <c r="K16" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="L16" s="36" t="s">
+      <c r="L16" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36" t="s">
+      <c r="M16" s="25"/>
+      <c r="N16" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="O16" s="36"/>
+      <c r="O16" s="25"/>
     </row>
     <row r="17" spans="1:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15">
         <v>1</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
       <c r="K17" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="L17" s="24" t="s">
+      <c r="L17" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24" t="s">
+      <c r="M17" s="38"/>
+      <c r="N17" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O17" s="24"/>
+      <c r="O17" s="38"/>
     </row>
     <row r="18" spans="1:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15">
         <v>2</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
       <c r="K18" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="L18" s="24" t="s">
+      <c r="L18" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24" t="s">
+      <c r="M18" s="38"/>
+      <c r="N18" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="O18" s="24"/>
+      <c r="O18" s="38"/>
     </row>
     <row r="19" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
@@ -1188,15 +1191,15 @@
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
-      <c r="K19" s="30" t="s">
+      <c r="K19" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="24" t="s">
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="O19" s="24"/>
+      <c r="O19" s="38"/>
     </row>
     <row r="20" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
@@ -1209,26 +1212,26 @@
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
-      <c r="K20" s="30" t="s">
+      <c r="K20" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="24" t="s">
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="O20" s="24"/>
+      <c r="O20" s="38"/>
     </row>
     <row r="21" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K21" s="30" t="s">
+      <c r="K21" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="24" t="s">
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="O21" s="24"/>
+      <c r="O21" s="38"/>
     </row>
     <row r="22" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K22" s="21"/>
@@ -1263,99 +1266,107 @@
         <v>23</v>
       </c>
       <c r="B26" s="26"/>
-      <c r="C26" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="46"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
+      <c r="C26" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="26"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B28" s="26"/>
-      <c r="C28" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="31" t="s">
+      <c r="C28" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="26"/>
       <c r="B29" s="26"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="26"/>
-      <c r="C30" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="31" t="s">
+      <c r="C30" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="26"/>
       <c r="B31" s="26"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="33" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="2"/>
@@ -1365,7 +1376,7 @@
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="26"/>
       <c r="B33" s="26"/>
-      <c r="C33" s="28"/>
+      <c r="C33" s="34"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -1452,7 +1463,30 @@
       <c r="P37" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="34">
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="D26:O27"/>
+    <mergeCell ref="A32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="D30:J31"/>
+    <mergeCell ref="D28:J29"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="A26:B27"/>
+    <mergeCell ref="A28:B29"/>
+    <mergeCell ref="C28:C29"/>
     <mergeCell ref="A1:G6"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="N16:O16"/>
@@ -1463,31 +1497,7 @@
     <mergeCell ref="A14:N15"/>
     <mergeCell ref="K11:O12"/>
     <mergeCell ref="K9:O9"/>
-    <mergeCell ref="A32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="D30:J31"/>
-    <mergeCell ref="D28:J29"/>
-    <mergeCell ref="D26:J27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A26:B27"/>
-    <mergeCell ref="A28:B29"/>
-    <mergeCell ref="C28:C29"/>
     <mergeCell ref="B10:G10"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="L26:O26"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K6" r:id="rId1" xr:uid="{6315ACE1-7DF9-479D-91B1-1F48D93FF882}"/>
@@ -1524,28 +1534,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
       <c r="H1" s="7"/>
       <c r="K1" s="17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="7"/>
       <c r="I2" s="1" t="s">
         <v>0</v>
@@ -1558,26 +1568,26 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="7"/>
       <c r="K3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="7"/>
       <c r="I4" s="1" t="s">
         <v>4</v>
@@ -1590,13 +1600,13 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="7"/>
       <c r="I5" s="1" t="s">
         <v>6</v>
@@ -1609,13 +1619,13 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="7"/>
       <c r="I6" s="1" t="s">
         <v>8</v>
@@ -1628,15 +1638,15 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="4"/>
       <c r="I7" s="1" t="s">
         <v>10</v>
@@ -1656,13 +1666,13 @@
       <c r="J9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K9" s="40" t="s">
+      <c r="K9" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
@@ -1690,7 +1700,7 @@
       <c r="I11" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="37" t="s">
+      <c r="J11" s="27" t="s">
         <v>1</v>
       </c>
       <c r="K11" s="26" t="s">
@@ -1711,12 +1721,12 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="26"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
@@ -1729,119 +1739,119 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
     </row>
     <row r="15" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
     </row>
     <row r="16" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
       <c r="K16" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="L16" s="36" t="s">
+      <c r="L16" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36" t="s">
+      <c r="M16" s="25"/>
+      <c r="N16" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="O16" s="36"/>
+      <c r="O16" s="25"/>
     </row>
     <row r="17" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16">
         <v>1</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="45"/>
       <c r="K17" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="L17" s="24" t="s">
+      <c r="L17" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24" t="s">
+      <c r="M17" s="38"/>
+      <c r="N17" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="O17" s="24"/>
+      <c r="O17" s="38"/>
     </row>
     <row r="18" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16">
         <v>2</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="45"/>
       <c r="K18" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="L18" s="24" t="s">
+      <c r="L18" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24" t="s">
+      <c r="M18" s="38"/>
+      <c r="N18" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="O18" s="24"/>
+      <c r="O18" s="38"/>
     </row>
     <row r="19" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
@@ -1857,8 +1867,8 @@
       <c r="K19" s="26"/>
       <c r="L19" s="26"/>
       <c r="M19" s="26"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
     </row>
     <row r="20" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
@@ -1871,18 +1881,18 @@
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
     </row>
     <row r="21" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="29"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
     </row>
     <row r="22" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K22" s="19"/>
@@ -1896,21 +1906,21 @@
         <v>23</v>
       </c>
       <c r="B23" s="26"/>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="35" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="26"/>
       <c r="B24" s="26"/>
-      <c r="C24" s="28"/>
+      <c r="C24" s="34"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
@@ -1924,58 +1934,58 @@
         <v>24</v>
       </c>
       <c r="B25" s="26"/>
-      <c r="C25" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="31" t="s">
+      <c r="C25" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="26"/>
       <c r="B26" s="26"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="26"/>
-      <c r="C27" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="31" t="s">
+      <c r="C27" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="26"/>
       <c r="B28" s="26"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
       <c r="J28" s="10"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
@@ -1983,7 +1993,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="26"/>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="33" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="2"/>
@@ -1993,7 +2003,7 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="26"/>
       <c r="B30" s="26"/>
-      <c r="C30" s="28"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
@@ -2081,6 +2091,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A14:N15"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="A1:G6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="N21:O21"/>
     <mergeCell ref="A29:B30"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="K9:O9"/>
@@ -2097,23 +2124,6 @@
     <mergeCell ref="A27:B28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="K19:M19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="A14:N15"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="A1:G6"/>
-    <mergeCell ref="A7:G7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K6" r:id="rId1" xr:uid="{3C795343-1380-435C-A59C-C1E46405255E}"/>

</xml_diff>